<commit_message>
fix shark double counts
</commit_message>
<xml_diff>
--- a/output/aggregate_tables/Area Statistics/area_47_summary.xlsx
+++ b/output/aggregate_tables/Area Statistics/area_47_summary.xlsx
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C3" s="4" t="n">
-        <v>0.5350936836970592</v>
+        <v>0.5344385436970592</v>
       </c>
     </row>
     <row r="4">
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.6208532235478056</v>
+        <v>0.6201980835478056</v>
       </c>
     </row>
     <row r="6">
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>6.338331535448821</v>
+        <v>6.341402055340052</v>
       </c>
     </row>
     <row r="8">
@@ -1424,7 +1424,7 @@
         </is>
       </c>
       <c r="C8" s="4" t="n">
-        <v>39.54780046277306</v>
+        <v>39.51851520369351</v>
       </c>
     </row>
     <row r="9">
@@ -1435,7 +1435,7 @@
         </is>
       </c>
       <c r="C9" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
     </row>
     <row r="10">
@@ -1446,7 +1446,7 @@
         </is>
       </c>
       <c r="C10" s="4" t="n">
-        <v>45.88613199822188</v>
+        <v>45.85991725903357</v>
       </c>
     </row>
     <row r="11">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="C11" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
     </row>
   </sheetData>
@@ -1582,31 +1582,31 @@
         <v>0.08575953985074626</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0.5350936836970592</v>
+        <v>0.5344385436970592</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.7321769764521945</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.6208532235478056</v>
+        <v>0.6201980835478056</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>0.7321769764521945</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>6.338331535448821</v>
+        <v>6.341402055340052</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>39.54780046277306</v>
+        <v>39.51851520369351</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
       <c r="J4" s="4" t="n">
-        <v>45.88613199822188</v>
+        <v>45.85991725903357</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
     </row>
     <row r="5">
@@ -1619,31 +1619,31 @@
         <v>0.08575953985074626</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.5350936836970592</v>
+        <v>0.5344385436970592</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>0.7321769764521945</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.6208532235478056</v>
+        <v>0.6201980835478056</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>0.7321769764521945</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>6.338331535448821</v>
+        <v>6.341402055340052</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>39.54780046277306</v>
+        <v>39.51851520369351</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>45.88613199822188</v>
+        <v>45.85991725903357</v>
       </c>
       <c r="K5" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
     </row>
     <row r="6">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="C2" s="4" t="n">
-        <v>95.4277012277519</v>
+        <v>95.38283744105355</v>
       </c>
     </row>
     <row r="3">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="C3" s="4" t="n">
-        <v>6.338331535448821</v>
+        <v>6.341402055340052</v>
       </c>
     </row>
     <row r="4">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>39.54780046277306</v>
+        <v>39.51851520369351</v>
       </c>
     </row>
     <row r="5">
@@ -1741,7 +1741,7 @@
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
     </row>
     <row r="6">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>45.88613199822188</v>
+        <v>45.85991725903357</v>
       </c>
     </row>
     <row r="7">
@@ -1763,7 +1763,7 @@
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>54.11386800177811</v>
+        <v>54.14008274096643</v>
       </c>
     </row>
     <row r="8">

</xml_diff>